<commit_message>
RTM -TS -TC added
</commit_message>
<xml_diff>
--- a/RTM_All_Modules.xlsx
+++ b/RTM_All_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90E72022-C6E0-49F7-B724-EA42356D6F45}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C72E2B6-A0A8-44D7-97DF-E5D1A554B28E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="180">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -1159,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE34CF0-8890-43A6-9D70-4DB6854C32E2}">
   <dimension ref="A3:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39:E57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,9 +1209,6 @@
       <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1226,9 +1223,6 @@
       <c r="D5" t="s">
         <v>64</v>
       </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1243,9 +1237,6 @@
       <c r="D6" t="s">
         <v>67</v>
       </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1260,9 +1251,6 @@
       <c r="D7" t="s">
         <v>70</v>
       </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1277,9 +1265,6 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1294,9 +1279,6 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1311,9 +1293,6 @@
       <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1328,9 +1307,6 @@
       <c r="D11" t="s">
         <v>74</v>
       </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1345,9 +1321,6 @@
       <c r="D12" t="s">
         <v>77</v>
       </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1362,9 +1335,6 @@
       <c r="D13" t="s">
         <v>80</v>
       </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1379,9 +1349,6 @@
       <c r="D14" t="s">
         <v>83</v>
       </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1396,9 +1363,6 @@
       <c r="D15" t="s">
         <v>87</v>
       </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1413,11 +1377,8 @@
       <c r="D16" t="s">
         <v>90</v>
       </c>
-      <c r="F16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -1430,11 +1391,8 @@
       <c r="D17" t="s">
         <v>93</v>
       </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>94</v>
       </c>
@@ -1447,11 +1405,8 @@
       <c r="D18" t="s">
         <v>96</v>
       </c>
-      <c r="F18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -1464,11 +1419,8 @@
       <c r="D19" t="s">
         <v>98</v>
       </c>
-      <c r="F19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1481,11 +1433,8 @@
       <c r="D20" t="s">
         <v>20</v>
       </c>
-      <c r="F20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -1498,11 +1447,8 @@
       <c r="D21" t="s">
         <v>103</v>
       </c>
-      <c r="F21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -1515,11 +1461,8 @@
       <c r="D22" t="s">
         <v>106</v>
       </c>
-      <c r="F22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>107</v>
       </c>
@@ -1532,11 +1475,8 @@
       <c r="D23" t="s">
         <v>109</v>
       </c>
-      <c r="F23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -1549,11 +1489,8 @@
       <c r="D24" t="s">
         <v>111</v>
       </c>
-      <c r="F24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1566,11 +1503,8 @@
       <c r="D25" t="s">
         <v>25</v>
       </c>
-      <c r="F25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1583,11 +1517,8 @@
       <c r="D26" t="s">
         <v>29</v>
       </c>
-      <c r="F26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>115</v>
       </c>
@@ -1600,11 +1531,8 @@
       <c r="D27" t="s">
         <v>117</v>
       </c>
-      <c r="F27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>118</v>
       </c>
@@ -1617,11 +1545,8 @@
       <c r="D28" t="s">
         <v>120</v>
       </c>
-      <c r="F28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -1634,11 +1559,8 @@
       <c r="D29" t="s">
         <v>122</v>
       </c>
-      <c r="F29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1651,11 +1573,8 @@
       <c r="D30" t="s">
         <v>34</v>
       </c>
-      <c r="F30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>125</v>
       </c>
@@ -1668,11 +1587,8 @@
       <c r="D31" t="s">
         <v>127</v>
       </c>
-      <c r="F31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>128</v>
       </c>
@@ -1685,11 +1601,8 @@
       <c r="D32" t="s">
         <v>130</v>
       </c>
-      <c r="F32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -1702,11 +1615,8 @@
       <c r="D33" t="s">
         <v>133</v>
       </c>
-      <c r="F33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>134</v>
       </c>
@@ -1719,11 +1629,8 @@
       <c r="D34" t="s">
         <v>135</v>
       </c>
-      <c r="F34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1736,11 +1643,8 @@
       <c r="D35" t="s">
         <v>39</v>
       </c>
-      <c r="F35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -1753,11 +1657,8 @@
       <c r="D36" t="s">
         <v>139</v>
       </c>
-      <c r="F36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>140</v>
       </c>
@@ -1770,11 +1671,8 @@
       <c r="D37" t="s">
         <v>142</v>
       </c>
-      <c r="F37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -1787,11 +1685,8 @@
       <c r="D38" t="s">
         <v>144</v>
       </c>
-      <c r="F38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1804,11 +1699,8 @@
       <c r="D39" t="s">
         <v>44</v>
       </c>
-      <c r="F39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1821,11 +1713,8 @@
       <c r="D40" t="s">
         <v>48</v>
       </c>
-      <c r="F40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -1838,11 +1727,8 @@
       <c r="D41" t="s">
         <v>150</v>
       </c>
-      <c r="F41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -1855,11 +1741,8 @@
       <c r="D42" t="s">
         <v>153</v>
       </c>
-      <c r="F42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>154</v>
       </c>
@@ -1872,11 +1755,8 @@
       <c r="D43" t="s">
         <v>156</v>
       </c>
-      <c r="F43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>157</v>
       </c>
@@ -1889,11 +1769,8 @@
       <c r="D44" t="s">
         <v>158</v>
       </c>
-      <c r="F44" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -1906,11 +1783,8 @@
       <c r="D45" t="s">
         <v>44</v>
       </c>
-      <c r="F45" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1923,11 +1797,8 @@
       <c r="D46" t="s">
         <v>48</v>
       </c>
-      <c r="F46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>148</v>
       </c>
@@ -1940,11 +1811,8 @@
       <c r="D47" t="s">
         <v>150</v>
       </c>
-      <c r="F47" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>151</v>
       </c>
@@ -1957,11 +1825,8 @@
       <c r="D48" t="s">
         <v>153</v>
       </c>
-      <c r="F48" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>154</v>
       </c>
@@ -1974,11 +1839,8 @@
       <c r="D49" t="s">
         <v>156</v>
       </c>
-      <c r="F49" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>157</v>
       </c>
@@ -1991,11 +1853,8 @@
       <c r="D50" t="s">
         <v>158</v>
       </c>
-      <c r="F50" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>159</v>
       </c>
@@ -2008,11 +1867,8 @@
       <c r="D51" t="s">
         <v>162</v>
       </c>
-      <c r="F51" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>163</v>
       </c>
@@ -2025,11 +1881,8 @@
       <c r="D52" t="s">
         <v>165</v>
       </c>
-      <c r="F52" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>166</v>
       </c>
@@ -2042,11 +1895,8 @@
       <c r="D53" t="s">
         <v>168</v>
       </c>
-      <c r="F53" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>169</v>
       </c>
@@ -2059,11 +1909,8 @@
       <c r="D54" t="s">
         <v>171</v>
       </c>
-      <c r="F54" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>172</v>
       </c>
@@ -2076,11 +1923,8 @@
       <c r="D55" t="s">
         <v>174</v>
       </c>
-      <c r="F55" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -2093,11 +1937,8 @@
       <c r="D56" t="s">
         <v>176</v>
       </c>
-      <c r="F56" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>177</v>
       </c>
@@ -2109,9 +1950,6 @@
       </c>
       <c r="D57" t="s">
         <v>179</v>
-      </c>
-      <c r="F57" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TC for Product search added
</commit_message>
<xml_diff>
--- a/RTM_All_Modules.xlsx
+++ b/RTM_All_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F5316D8-1C73-4278-B64D-DB4A2C9E2DAD}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{153927AF-ED9A-47EF-8F5B-1108443DB0F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="204">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -376,28 +376,16 @@
     <t>TS_SEARCH_05</t>
   </si>
   <si>
-    <t>Add products to cart</t>
-  </si>
-  <si>
     <t>Add to Cart</t>
   </si>
   <si>
-    <t>Update quantity in cart</t>
-  </si>
-  <si>
     <t>FR_CART_03</t>
   </si>
   <si>
-    <t>Remove products from cart</t>
-  </si>
-  <si>
     <t>TS_CART_03</t>
   </si>
   <si>
     <t>FR_CART_04</t>
-  </si>
-  <si>
-    <t>Correct total price calculation</t>
   </si>
   <si>
     <t>TS_CART_04</t>
@@ -646,6 +634,21 @@
   </si>
   <si>
     <t>TS_REG_07</t>
+  </si>
+  <si>
+    <t>FR_CART_06</t>
+  </si>
+  <si>
+    <t>User should be able to add product to cart</t>
+  </si>
+  <si>
+    <t>User should be able to update product quantity</t>
+  </si>
+  <si>
+    <t>Cart should show correct total price</t>
+  </si>
+  <si>
+    <t>TS_CART_06</t>
   </si>
 </sst>
 </file>
@@ -1257,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE34CF0-8890-43A6-9D70-4DB6854C32E2}">
-  <dimension ref="A3:G63"/>
+  <dimension ref="A3:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,10 +1313,10 @@
         <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1330,10 +1333,10 @@
         <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1353,7 +1356,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1370,10 +1373,10 @@
         <v>71</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1476,86 +1479,86 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B15" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C15" t="s">
         <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C16" t="s">
         <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B17" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C17" t="s">
         <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C18" t="s">
         <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C19" t="s">
         <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B20" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C20" t="s">
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1703,10 +1706,10 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
+        <v>200</v>
+      </c>
+      <c r="C31" t="s">
         <v>113</v>
-      </c>
-      <c r="C31" t="s">
-        <v>114</v>
       </c>
       <c r="D31" t="s">
         <v>25</v>
@@ -1717,10 +1720,10 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
         <v>29</v>
@@ -1728,439 +1731,454 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>201</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>201</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>202</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>199</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>202</v>
       </c>
       <c r="C36" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>34</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D37" t="s">
-        <v>128</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C38" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C39" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="D41" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C42" t="s">
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>138</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="B45" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C46" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D47" t="s">
-        <v>151</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B48" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" t="s">
         <v>147</v>
-      </c>
-      <c r="D48" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B49" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C49" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D49" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D50" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D51" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D52" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>149</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C53" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D53" t="s">
-        <v>151</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C54" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" t="s">
         <v>147</v>
-      </c>
-      <c r="D54" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C55" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D55" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="C56" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D56" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D57" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B58" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C58" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D58" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B59" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C59" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59" t="s">
         <v>162</v>
-      </c>
-      <c r="D59" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B60" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C60" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D60" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B61" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C61" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D61" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>170</v>
       </c>
       <c r="C62" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D62" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B63" t="s">
-        <v>179</v>
+        <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D63" t="s">
-        <v>180</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>174</v>
+      </c>
+      <c r="B64" t="s">
+        <v>175</v>
+      </c>
+      <c r="C64" t="s">
+        <v>158</v>
+      </c>
+      <c r="D64" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2239,10 +2257,10 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E18" t="s">
         <v>74</v>
@@ -2250,10 +2268,10 @@
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E19" t="s">
         <v>74</v>
@@ -2261,10 +2279,10 @@
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E20" t="s">
         <v>74</v>
@@ -2272,10 +2290,10 @@
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D21" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E21" t="s">
         <v>74</v>
@@ -2283,10 +2301,10 @@
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D22" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E22" t="s">
         <v>74</v>
@@ -2294,10 +2312,10 @@
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D23" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E23" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
TC for checkout added
</commit_message>
<xml_diff>
--- a/RTM_All_Modules.xlsx
+++ b/RTM_All_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{153927AF-ED9A-47EF-8F5B-1108443DB0F7}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3360056-3CBB-4E21-844D-D89B6CA9428F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="209">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -422,9 +422,6 @@
   </si>
   <si>
     <t>FR_CHECKOUT_04</t>
-  </si>
-  <si>
-    <t>Display order summary correctly</t>
   </si>
   <si>
     <t>TS_CHECKOUT_04</t>
@@ -649,6 +646,24 @@
   </si>
   <si>
     <t>TS_CART_06</t>
+  </si>
+  <si>
+    <t>FR_CHECKOUT_06</t>
+  </si>
+  <si>
+    <t>FR_CHECKOUT_07</t>
+  </si>
+  <si>
+    <t>Select exiting delivery address</t>
+  </si>
+  <si>
+    <t>Add/remove address</t>
+  </si>
+  <si>
+    <t>Check delivery option</t>
+  </si>
+  <si>
+    <t>Check the payment option</t>
   </si>
 </sst>
 </file>
@@ -1260,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE34CF0-8890-43A6-9D70-4DB6854C32E2}">
-  <dimension ref="A3:G64"/>
+  <dimension ref="A3:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35:D36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,10 +1328,10 @@
         <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,10 +1348,10 @@
         <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,7 +1371,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1373,10 +1388,10 @@
         <v>71</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1479,86 +1494,86 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
         <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C16" t="s">
         <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C17" t="s">
         <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C18" t="s">
         <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" t="s">
         <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C20" t="s">
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1706,7 +1721,7 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C31" t="s">
         <v>113</v>
@@ -1720,7 +1735,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" t="s">
         <v>113</v>
@@ -1734,7 +1749,7 @@
         <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" t="s">
         <v>113</v>
@@ -1748,7 +1763,7 @@
         <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" t="s">
         <v>113</v>
@@ -1762,7 +1777,7 @@
         <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C35" t="s">
         <v>113</v>
@@ -1773,16 +1788,16 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C36" t="s">
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1804,7 +1819,7 @@
         <v>122</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C38" t="s">
         <v>121</v>
@@ -1818,7 +1833,7 @@
         <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C39" t="s">
         <v>121</v>
@@ -1832,349 +1847,371 @@
         <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
+        <v>205</v>
       </c>
       <c r="C40" t="s">
         <v>121</v>
       </c>
       <c r="D40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>206</v>
       </c>
       <c r="C41" t="s">
         <v>121</v>
       </c>
       <c r="D41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>203</v>
       </c>
       <c r="B42" t="s">
-        <v>133</v>
+        <v>207</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" t="s">
-        <v>39</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>208</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
-      </c>
-      <c r="D43" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="B46" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C46" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="B47" t="s">
-        <v>144</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D48" t="s">
-        <v>147</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D49" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>150</v>
       </c>
       <c r="B52" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" t="s">
         <v>142</v>
       </c>
-      <c r="C52" t="s">
-        <v>143</v>
-      </c>
       <c r="D52" t="s">
-        <v>44</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D53" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>41</v>
       </c>
       <c r="B54" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D54" t="s">
-        <v>147</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D55" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B56" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D56" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="C57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D57" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="D58" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
-        <v>161</v>
+        <v>63</v>
       </c>
       <c r="C59" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="D59" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B60" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C60" t="s">
+        <v>157</v>
+      </c>
+      <c r="D60" t="s">
         <v>158</v>
-      </c>
-      <c r="D60" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B61" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C61" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D61" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B62" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D62" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="C63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D63" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" t="s">
+        <v>169</v>
+      </c>
+      <c r="C64" t="s">
+        <v>157</v>
+      </c>
+      <c r="D64" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>171</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" t="s">
+        <v>157</v>
+      </c>
+      <c r="D65" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" t="s">
         <v>174</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C66" t="s">
+        <v>157</v>
+      </c>
+      <c r="D66" t="s">
         <v>175</v>
-      </c>
-      <c r="C64" t="s">
-        <v>158</v>
-      </c>
-      <c r="D64" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2257,10 +2294,10 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E18" t="s">
         <v>74</v>
@@ -2268,10 +2305,10 @@
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E19" t="s">
         <v>74</v>
@@ -2279,10 +2316,10 @@
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E20" t="s">
         <v>74</v>
@@ -2290,10 +2327,10 @@
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E21" t="s">
         <v>74</v>
@@ -2301,10 +2338,10 @@
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E22" t="s">
         <v>74</v>
@@ -2312,10 +2349,10 @@
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E23" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
TC for order added
</commit_message>
<xml_diff>
--- a/RTM_All_Modules.xlsx
+++ b/RTM_All_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DD4FF57-DE0A-4B0D-A229-704BFD0CF6A7}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88952B13-BD3B-4020-A01D-F1506F8AFD5C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="223">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -466,25 +466,16 @@
     <t>FR_ORDER_03</t>
   </si>
   <si>
-    <t>Order details in My Orders</t>
-  </si>
-  <si>
     <t>TS_ORDER_03</t>
   </si>
   <si>
     <t>FR_ORDER_04</t>
   </si>
   <si>
-    <t>Order tracking functionality</t>
-  </si>
-  <si>
     <t>TS_ORDER_04</t>
   </si>
   <si>
     <t>FR_ORDER_05</t>
-  </si>
-  <si>
-    <t>Order cancellation before shipment</t>
   </si>
   <si>
     <t>TS_ORDER_05</t>
@@ -697,6 +688,24 @@
   </si>
   <si>
     <t>Secure paymnet</t>
+  </si>
+  <si>
+    <t>FR_ORDER_07</t>
+  </si>
+  <si>
+    <t>Order details in display</t>
+  </si>
+  <si>
+    <t>Payment status should be shown</t>
+  </si>
+  <si>
+    <t>Order confirmation message should be displayed</t>
+  </si>
+  <si>
+    <t>Order details should be available in “My Orders”</t>
+  </si>
+  <si>
+    <t>Confirmation email/SMS should be sent</t>
   </si>
 </sst>
 </file>
@@ -1308,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE34CF0-8890-43A6-9D70-4DB6854C32E2}">
-  <dimension ref="A3:G69"/>
+  <dimension ref="A3:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,10 +1370,10 @@
         <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1381,10 +1390,10 @@
         <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1404,7 +1413,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1421,10 +1430,10 @@
         <v>71</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1527,86 +1536,86 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C15" t="s">
         <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C16" t="s">
         <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C17" t="s">
         <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C18" t="s">
         <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C19" t="s">
         <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C20" t="s">
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1768,7 +1777,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C32" t="s">
         <v>113</v>
@@ -1782,7 +1791,7 @@
         <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C33" t="s">
         <v>113</v>
@@ -1796,7 +1805,7 @@
         <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C34" t="s">
         <v>113</v>
@@ -1810,7 +1819,7 @@
         <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C35" t="s">
         <v>113</v>
@@ -1821,16 +1830,16 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B36" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C36" t="s">
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1880,7 +1889,7 @@
         <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C40" t="s">
         <v>121</v>
@@ -1894,7 +1903,7 @@
         <v>130</v>
       </c>
       <c r="B41" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C41" t="s">
         <v>121</v>
@@ -1905,30 +1914,30 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B42" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C42" t="s">
         <v>121</v>
       </c>
       <c r="D42" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B43" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C43" t="s">
         <v>121</v>
       </c>
       <c r="D43" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1950,7 +1959,7 @@
         <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
@@ -1964,7 +1973,7 @@
         <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C46" t="s">
         <v>38</v>
@@ -1978,7 +1987,7 @@
         <v>137</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
@@ -1989,10 +1998,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B48" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
@@ -2000,10 +2009,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B49" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
@@ -2011,10 +2020,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B50" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
@@ -2025,7 +2034,7 @@
         <v>41</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C51" t="s">
         <v>140</v>
@@ -2039,7 +2048,7 @@
         <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C52" t="s">
         <v>140</v>
@@ -2053,237 +2062,164 @@
         <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>143</v>
+        <v>218</v>
       </c>
       <c r="C53" t="s">
         <v>140</v>
       </c>
       <c r="D53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B54" t="s">
-        <v>146</v>
+        <v>219</v>
       </c>
       <c r="C54" t="s">
         <v>140</v>
       </c>
       <c r="D54" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B55" t="s">
-        <v>149</v>
+        <v>220</v>
       </c>
       <c r="C55" t="s">
         <v>140</v>
       </c>
       <c r="D55" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>221</v>
       </c>
       <c r="C56" t="s">
         <v>140</v>
       </c>
       <c r="D56" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>217</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>222</v>
       </c>
       <c r="C57" t="s">
         <v>140</v>
       </c>
-      <c r="D57" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D58" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D59" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="B60" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="C60" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D60" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="B61" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D61" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>164</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D62" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="B63" t="s">
-        <v>154</v>
+        <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D63" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B64" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C64" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D64" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>160</v>
-      </c>
-      <c r="B65" t="s">
-        <v>161</v>
-      </c>
-      <c r="C65" t="s">
-        <v>155</v>
-      </c>
-      <c r="D65" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>163</v>
-      </c>
-      <c r="B66" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" t="s">
-        <v>155</v>
-      </c>
-      <c r="D66" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>166</v>
-      </c>
-      <c r="B67" t="s">
-        <v>167</v>
-      </c>
-      <c r="C67" t="s">
-        <v>155</v>
-      </c>
-      <c r="D67" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>169</v>
-      </c>
-      <c r="B68" t="s">
-        <v>63</v>
-      </c>
-      <c r="C68" t="s">
-        <v>155</v>
-      </c>
-      <c r="D68" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>171</v>
-      </c>
-      <c r="B69" t="s">
-        <v>172</v>
-      </c>
-      <c r="C69" t="s">
-        <v>155</v>
-      </c>
-      <c r="D69" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2367,10 +2303,10 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E18" t="s">
         <v>74</v>
@@ -2378,10 +2314,10 @@
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E19" t="s">
         <v>74</v>
@@ -2389,10 +2325,10 @@
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E20" t="s">
         <v>74</v>
@@ -2400,10 +2336,10 @@
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E21" t="s">
         <v>74</v>
@@ -2411,10 +2347,10 @@
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D22" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E22" t="s">
         <v>74</v>
@@ -2422,10 +2358,10 @@
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D23" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E23" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
TC for non functional added
</commit_message>
<xml_diff>
--- a/RTM_All_Modules.xlsx
+++ b/RTM_All_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9865239-5809-4789-9EC7-861CCC179F71}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38AC752E-2CEE-4986-9491-56A9F856E511}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -490,9 +490,6 @@
     <t>NFR_01</t>
   </si>
   <si>
-    <t>Pages load within 3 seconds</t>
-  </si>
-  <si>
     <t>Non-Functional</t>
   </si>
   <si>
@@ -502,36 +499,24 @@
     <t>NFR_02</t>
   </si>
   <si>
-    <t>User-friendly UI</t>
-  </si>
-  <si>
     <t>TS_NFR_02</t>
   </si>
   <si>
     <t>NFR_03</t>
   </si>
   <si>
-    <t>Meaningful error messages</t>
-  </si>
-  <si>
     <t>TS_NFR_03</t>
   </si>
   <si>
     <t>NFR_04</t>
   </si>
   <si>
-    <t>Password masking &amp; secure data</t>
-  </si>
-  <si>
     <t>TS_NFR_04</t>
   </si>
   <si>
     <t>NFR_05</t>
   </si>
   <si>
-    <t>Restrict unauthorized access</t>
-  </si>
-  <si>
     <t>TS_NFR_05</t>
   </si>
   <si>
@@ -542,9 +527,6 @@
   </si>
   <si>
     <t>NFR_07</t>
-  </si>
-  <si>
-    <t>Responsive design</t>
   </si>
   <si>
     <t>TS_NFR_07</t>
@@ -772,6 +754,24 @@
   </si>
   <si>
     <t>TS_OT_06</t>
+  </si>
+  <si>
+    <t>Application performance</t>
+  </si>
+  <si>
+    <t>Application usability</t>
+  </si>
+  <si>
+    <t>Application security</t>
+  </si>
+  <si>
+    <t>Application reliability</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Data integrity</t>
   </si>
 </sst>
 </file>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE34CF0-8890-43A6-9D70-4DB6854C32E2}">
   <dimension ref="A3:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,10 +1436,10 @@
         <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1456,10 +1456,10 @@
         <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1496,10 +1496,10 @@
         <v>71</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1602,86 +1602,86 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
         <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
         <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C17" t="s">
         <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C18" t="s">
         <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B19" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C19" t="s">
         <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C20" t="s">
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1843,7 +1843,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C32" t="s">
         <v>113</v>
@@ -1857,7 +1857,7 @@
         <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C33" t="s">
         <v>113</v>
@@ -1871,7 +1871,7 @@
         <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C34" t="s">
         <v>113</v>
@@ -1885,7 +1885,7 @@
         <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C35" t="s">
         <v>113</v>
@@ -1896,16 +1896,16 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B36" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C36" t="s">
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,7 +1955,7 @@
         <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C40" t="s">
         <v>121</v>
@@ -1969,7 +1969,7 @@
         <v>130</v>
       </c>
       <c r="B41" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C41" t="s">
         <v>121</v>
@@ -1980,30 +1980,30 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B42" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C42" t="s">
         <v>121</v>
       </c>
       <c r="D42" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B43" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C43" t="s">
         <v>121</v>
       </c>
       <c r="D43" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2025,7 +2025,7 @@
         <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
@@ -2039,7 +2039,7 @@
         <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C46" t="s">
         <v>38</v>
@@ -2053,7 +2053,7 @@
         <v>137</v>
       </c>
       <c r="B47" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
@@ -2064,44 +2064,44 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>202</v>
+      </c>
+      <c r="B48" t="s">
         <v>208</v>
-      </c>
-      <c r="B48" t="s">
-        <v>214</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>203</v>
+      </c>
+      <c r="B49" t="s">
         <v>209</v>
-      </c>
-      <c r="B49" t="s">
-        <v>215</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>204</v>
+      </c>
+      <c r="B50" t="s">
         <v>210</v>
-      </c>
-      <c r="B50" t="s">
-        <v>216</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2137,7 +2137,7 @@
         <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C53" t="s">
         <v>140</v>
@@ -2151,7 +2151,7 @@
         <v>144</v>
       </c>
       <c r="B54" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C54" t="s">
         <v>140</v>
@@ -2165,7 +2165,7 @@
         <v>146</v>
       </c>
       <c r="B55" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C55" t="s">
         <v>140</v>
@@ -2179,7 +2179,7 @@
         <v>148</v>
       </c>
       <c r="B56" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C56" t="s">
         <v>140</v>
@@ -2190,100 +2190,100 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B57" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C57" t="s">
         <v>140</v>
       </c>
       <c r="D57" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>221</v>
+      </c>
+      <c r="B58" t="s">
         <v>227</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
+        <v>232</v>
+      </c>
+      <c r="D58" t="s">
         <v>233</v>
-      </c>
-      <c r="C58" t="s">
-        <v>238</v>
-      </c>
-      <c r="D58" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>222</v>
+      </c>
+      <c r="B59" t="s">
         <v>228</v>
       </c>
-      <c r="B59" t="s">
-        <v>234</v>
-      </c>
       <c r="C59" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D59" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>223</v>
+      </c>
+      <c r="B60" t="s">
         <v>229</v>
       </c>
-      <c r="B60" t="s">
-        <v>235</v>
-      </c>
       <c r="C60" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D60" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>224</v>
+      </c>
+      <c r="B61" t="s">
         <v>230</v>
       </c>
-      <c r="B61" t="s">
-        <v>236</v>
-      </c>
       <c r="C61" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D61" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>225</v>
+      </c>
+      <c r="B62" t="s">
         <v>231</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
+        <v>232</v>
+      </c>
+      <c r="D62" t="s">
         <v>237</v>
-      </c>
-      <c r="C62" t="s">
-        <v>238</v>
-      </c>
-      <c r="D62" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>226</v>
+      </c>
+      <c r="B63" t="s">
+        <v>231</v>
+      </c>
+      <c r="C63" t="s">
         <v>232</v>
       </c>
-      <c r="B63" t="s">
-        <v>237</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>238</v>
-      </c>
-      <c r="D63" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2291,97 +2291,97 @@
         <v>150</v>
       </c>
       <c r="B64" t="s">
+        <v>239</v>
+      </c>
+      <c r="C64" t="s">
         <v>151</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>152</v>
-      </c>
-      <c r="D64" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>153</v>
+      </c>
+      <c r="B65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C65" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" t="s">
         <v>154</v>
-      </c>
-      <c r="B65" t="s">
-        <v>155</v>
-      </c>
-      <c r="C65" t="s">
-        <v>152</v>
-      </c>
-      <c r="D65" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B66" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D66" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
-        <v>161</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D67" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B68" t="s">
-        <v>164</v>
+        <v>242</v>
       </c>
       <c r="C68" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D68" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B69" t="s">
-        <v>63</v>
+        <v>243</v>
       </c>
       <c r="C69" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D69" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B70" t="s">
-        <v>169</v>
+        <v>244</v>
       </c>
       <c r="C70" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D70" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2465,10 +2465,10 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E18" t="s">
         <v>74</v>
@@ -2476,10 +2476,10 @@
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E19" t="s">
         <v>74</v>
@@ -2487,10 +2487,10 @@
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E20" t="s">
         <v>74</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E21" t="s">
         <v>74</v>
@@ -2509,10 +2509,10 @@
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D22" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E22" t="s">
         <v>74</v>
@@ -2520,10 +2520,10 @@
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D23" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E23" t="s">
         <v>74</v>

</xml_diff>